<commit_message>
hardware v1.0. not tested
</commit_message>
<xml_diff>
--- a/fpga_asd_mapping.xlsx
+++ b/fpga_asd_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Documentos\Estudios\UTFSM\ELO308 - Memoria de Titulacion\Vivado\muon-daq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCC88CD-4658-4B3E-B5D5-402812D9A594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE41883E-33B8-4196-BEB7-AE0007189B56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="795" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{6A2EA7B9-2101-44CC-9935-C6BE564B6AF4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{6A2EA7B9-2101-44CC-9935-C6BE564B6AF4}"/>
   </bookViews>
   <sheets>
     <sheet name="TE0712" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="453">
   <si>
     <t>FPGA Pin</t>
   </si>
@@ -4063,8 +4063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39C874D-C1A1-4D3E-9D2B-D05BF72AF7EC}">
   <dimension ref="B2:O82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4134,8 +4134,9 @@
       <c r="F3" s="6">
         <v>0</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>4</v>
+      <c r="G3" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[0]</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>387</v>
@@ -4152,8 +4153,9 @@
       <c r="N3" s="2">
         <v>0</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>5</v>
+      <c r="O3" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[0]</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -4172,8 +4174,9 @@
       <c r="F4" s="6">
         <v>0</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>2</v>
+      <c r="G4" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[0]</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>388</v>
@@ -4190,8 +4193,9 @@
       <c r="N4" s="3">
         <v>0</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>15</v>
+      <c r="O4" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[0]</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
@@ -4210,8 +4214,9 @@
       <c r="F5" s="6">
         <v>1</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>17</v>
+      <c r="G5" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[1]</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>359</v>
@@ -4228,8 +4233,9 @@
       <c r="N5" s="2">
         <v>1</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>3</v>
+      <c r="O5" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[1]</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -4248,8 +4254,9 @@
       <c r="F6" s="6">
         <v>1</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>16</v>
+      <c r="G6" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[1]</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>360</v>
@@ -4266,8 +4273,9 @@
       <c r="N6" s="3">
         <v>1</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>43</v>
+      <c r="O6" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[1]</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -4286,8 +4294,9 @@
       <c r="F7" s="6">
         <v>2</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>80</v>
+      <c r="G7" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[2]</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>391</v>
@@ -4304,8 +4313,9 @@
       <c r="N7" s="2">
         <v>2</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>6</v>
+      <c r="O7" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[2]</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -4324,8 +4334,9 @@
       <c r="F8" s="6">
         <v>2</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>18</v>
+      <c r="G8" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[2]</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>392</v>
@@ -4342,8 +4353,9 @@
       <c r="N8" s="3">
         <v>2</v>
       </c>
-      <c r="O8" s="3" t="s">
-        <v>44</v>
+      <c r="O8" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[2]</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -4362,8 +4374,9 @@
       <c r="F9" s="6">
         <v>3</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>19</v>
+      <c r="G9" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[3]</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>363</v>
@@ -4380,8 +4393,9 @@
       <c r="N9" s="2">
         <v>3</v>
       </c>
-      <c r="O9" s="2" t="s">
-        <v>7</v>
+      <c r="O9" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[3]</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -4400,8 +4414,9 @@
       <c r="F10" s="6">
         <v>3</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>20</v>
+      <c r="G10" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[3]</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>364</v>
@@ -4418,8 +4433,9 @@
       <c r="N10" s="3">
         <v>3</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>45</v>
+      <c r="O10" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[3]</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
@@ -4438,8 +4454,9 @@
       <c r="F11" s="6">
         <v>4</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>21</v>
+      <c r="G11" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[4]</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>395</v>
@@ -4456,8 +4473,9 @@
       <c r="N11" s="2">
         <v>4</v>
       </c>
-      <c r="O11" s="2" t="s">
-        <v>8</v>
+      <c r="O11" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[4]</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
@@ -4476,8 +4494,9 @@
       <c r="F12" s="6">
         <v>4</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>22</v>
+      <c r="G12" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[4]</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>396</v>
@@ -4494,8 +4513,9 @@
       <c r="N12" s="3">
         <v>4</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>46</v>
+      <c r="O12" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[4]</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -4514,8 +4534,9 @@
       <c r="F13" s="6">
         <v>5</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>24</v>
+      <c r="G13" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[5]</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>367</v>
@@ -4532,8 +4553,9 @@
       <c r="N13" s="2">
         <v>5</v>
       </c>
-      <c r="O13" s="2" t="s">
-        <v>9</v>
+      <c r="O13" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[5]</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
@@ -4552,8 +4574,9 @@
       <c r="F14" s="6">
         <v>5</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>23</v>
+      <c r="G14" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[5]</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>368</v>
@@ -4570,8 +4593,9 @@
       <c r="N14" s="3">
         <v>5</v>
       </c>
-      <c r="O14" s="3" t="s">
-        <v>47</v>
+      <c r="O14" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[5]</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
@@ -4590,8 +4614,9 @@
       <c r="F15" s="6">
         <v>6</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>26</v>
+      <c r="G15" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[6]</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>400</v>
@@ -4608,8 +4633,9 @@
       <c r="N15" s="2">
         <v>6</v>
       </c>
-      <c r="O15" s="2" t="s">
-        <v>10</v>
+      <c r="O15" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[6]</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
@@ -4628,8 +4654,9 @@
       <c r="F16" s="6">
         <v>6</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>25</v>
+      <c r="G16" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[6]</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>398</v>
@@ -4646,8 +4673,9 @@
       <c r="N16" s="3">
         <v>6</v>
       </c>
-      <c r="O16" s="3" t="s">
-        <v>48</v>
+      <c r="O16" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[6]</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
@@ -4666,8 +4694,9 @@
       <c r="F17" s="6">
         <v>7</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>81</v>
+      <c r="G17" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[7]</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>354</v>
@@ -4684,8 +4713,9 @@
       <c r="N17" s="2">
         <v>7</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>11</v>
+      <c r="O17" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[7]</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
@@ -4704,8 +4734,9 @@
       <c r="F18" s="6">
         <v>7</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>27</v>
+      <c r="G18" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[7]</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>353</v>
@@ -4722,8 +4753,9 @@
       <c r="N18" s="3">
         <v>7</v>
       </c>
-      <c r="O18" s="3" t="s">
-        <v>49</v>
+      <c r="O18" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[7]</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
@@ -4742,8 +4774,9 @@
       <c r="F19" s="6">
         <v>8</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>28</v>
+      <c r="G19" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[8]</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>403</v>
@@ -4760,8 +4793,9 @@
       <c r="N19" s="2">
         <v>8</v>
       </c>
-      <c r="O19" s="2" t="s">
-        <v>12</v>
+      <c r="O19" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[8]</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
@@ -4780,8 +4814,9 @@
       <c r="F20" s="6">
         <v>8</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>29</v>
+      <c r="G20" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[8]</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>404</v>
@@ -4798,8 +4833,9 @@
       <c r="N20" s="3">
         <v>8</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>50</v>
+      <c r="O20" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[8]</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -4818,8 +4854,9 @@
       <c r="F21" s="6">
         <v>9</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>30</v>
+      <c r="G21" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[9]</v>
       </c>
       <c r="J21" s="2" t="s">
         <v>356</v>
@@ -4836,8 +4873,9 @@
       <c r="N21" s="2">
         <v>9</v>
       </c>
-      <c r="O21" s="2" t="s">
-        <v>13</v>
+      <c r="O21" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[9]</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
@@ -4856,8 +4894,9 @@
       <c r="F22" s="6">
         <v>9</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>31</v>
+      <c r="G22" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[9]</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>355</v>
@@ -4874,8 +4913,9 @@
       <c r="N22" s="3">
         <v>9</v>
       </c>
-      <c r="O22" s="3" t="s">
-        <v>51</v>
+      <c r="O22" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[9]</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -4894,8 +4934,9 @@
       <c r="F23" s="6">
         <v>10</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>33</v>
+      <c r="G23" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[10]</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>407</v>
@@ -4912,8 +4953,9 @@
       <c r="N23" s="2">
         <v>10</v>
       </c>
-      <c r="O23" s="2" t="s">
-        <v>14</v>
+      <c r="O23" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[10]</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
@@ -4932,8 +4974,9 @@
       <c r="F24" s="6">
         <v>10</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>32</v>
+      <c r="G24" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[10]</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>408</v>
@@ -4950,8 +4993,9 @@
       <c r="N24" s="3">
         <v>10</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>52</v>
+      <c r="O24" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[10]</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -4970,8 +5014,9 @@
       <c r="F25" s="6">
         <v>11</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>35</v>
+      <c r="G25" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[11]</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>375</v>
@@ -4988,8 +5033,9 @@
       <c r="N25" s="2">
         <v>11</v>
       </c>
-      <c r="O25" s="2" t="s">
-        <v>54</v>
+      <c r="O25" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[11]</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
@@ -5008,8 +5054,9 @@
       <c r="F26" s="6">
         <v>11</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>34</v>
+      <c r="G26" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[11]</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>376</v>
@@ -5026,8 +5073,9 @@
       <c r="N26" s="3">
         <v>11</v>
       </c>
-      <c r="O26" s="3" t="s">
-        <v>53</v>
+      <c r="O26" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[11]</v>
       </c>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
@@ -5046,8 +5094,9 @@
       <c r="F27" s="6">
         <v>12</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>82</v>
+      <c r="G27" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[12]</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>411</v>
@@ -5064,8 +5113,9 @@
       <c r="N27" s="2">
         <v>12</v>
       </c>
-      <c r="O27" s="2" t="s">
-        <v>56</v>
+      <c r="O27" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[12]</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
@@ -5084,8 +5134,9 @@
       <c r="F28" s="6">
         <v>12</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>36</v>
+      <c r="G28" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[12]</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>412</v>
@@ -5102,8 +5153,9 @@
       <c r="N28" s="3">
         <v>12</v>
       </c>
-      <c r="O28" s="3" t="s">
-        <v>55</v>
+      <c r="O28" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[12]</v>
       </c>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
@@ -5122,8 +5174,9 @@
       <c r="F29" s="6">
         <v>13</v>
       </c>
-      <c r="G29" s="6" t="s">
-        <v>38</v>
+      <c r="G29" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[13]</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>379</v>
@@ -5140,8 +5193,9 @@
       <c r="N29" s="2">
         <v>13</v>
       </c>
-      <c r="O29" s="2" t="s">
-        <v>58</v>
+      <c r="O29" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[13]</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
@@ -5160,8 +5214,9 @@
       <c r="F30" s="6">
         <v>13</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>37</v>
+      <c r="G30" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[13]</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>380</v>
@@ -5178,8 +5233,9 @@
       <c r="N30" s="3">
         <v>13</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>57</v>
+      <c r="O30" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[13]</v>
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
@@ -5198,8 +5254,9 @@
       <c r="F31" s="6">
         <v>14</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>40</v>
+      <c r="G31" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[14]</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>415</v>
@@ -5216,8 +5273,9 @@
       <c r="N31" s="2">
         <v>14</v>
       </c>
-      <c r="O31" s="2" t="s">
-        <v>61</v>
+      <c r="O31" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[14]</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
@@ -5236,8 +5294,9 @@
       <c r="F32" s="6">
         <v>14</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>39</v>
+      <c r="G32" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[14]</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>416</v>
@@ -5254,8 +5313,9 @@
       <c r="N32" s="3">
         <v>14</v>
       </c>
-      <c r="O32" s="3" t="s">
-        <v>59</v>
+      <c r="O32" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[14]</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
@@ -5274,8 +5334,9 @@
       <c r="F33" s="6">
         <v>15</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>42</v>
+      <c r="G33" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_P[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_P[15]</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>383</v>
@@ -5292,8 +5353,9 @@
       <c r="N33" s="2">
         <v>15</v>
       </c>
-      <c r="O33" s="2" t="s">
-        <v>60</v>
+      <c r="O33" s="2" t="str">
+        <f>_xlfn.CONCAT("Ch_B_P[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_P[15]</v>
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
@@ -5312,8 +5374,9 @@
       <c r="F34" s="6">
         <v>15</v>
       </c>
-      <c r="G34" s="6" t="s">
-        <v>41</v>
+      <c r="G34" s="6" t="str">
+        <f>_xlfn.CONCAT("Ch_A_N[",Tabla14[[#This Row],[Channel]],"]")</f>
+        <v>Ch_A_N[15]</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>384</v>
@@ -5330,229 +5393,230 @@
       <c r="N34" s="4">
         <v>15</v>
       </c>
-      <c r="O34" s="4" t="s">
-        <v>62</v>
+      <c r="O34" s="3" t="str">
+        <f>_xlfn.CONCAT("Ch_B_N[",Tabla25[[#This Row],[Channel]],"]")</f>
+        <v>Ch_B_N[15]</v>
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B3," IOSTANDARD LVDS_25} [get_ports ",G3,"]; #",C3)</f>
-        <v>set_property -dict {PACKAGE_PIN F16 IOSTANDARD LVDS_25} [get_ports Ch[0][0][1]]; #B35_L1_P</v>
+        <v>set_property -dict {PACKAGE_PIN F16 IOSTANDARD LVDS_25} [get_ports Ch_A_P[0]]; #B35_L1_P</v>
       </c>
       <c r="J36" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J3," IOSTANDARD LVDS_25} [get_ports ",O3,"]; #",K3)</f>
-        <v>set_property -dict {PACKAGE_PIN V5 IOSTANDARD LVDS_25} [get_ports Ch[1][0][1]]; #B13_L21_P</v>
+        <v>set_property -dict {PACKAGE_PIN V5 IOSTANDARD LVDS_25} [get_ports Ch_B_P[0]]; #B13_L21_P</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f t="shared" ref="B37" si="0">_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B4," IOSTANDARD LVDS_25} [get_ports ",G4,"]; #",C4)</f>
-        <v>set_property -dict {PACKAGE_PIN E16 IOSTANDARD LVDS_25} [get_ports Ch[0][0][0]]; #B35_L1_N</v>
+        <v>set_property -dict {PACKAGE_PIN E16 IOSTANDARD LVDS_25} [get_ports Ch_A_N[0]]; #B35_L1_N</v>
       </c>
       <c r="J37" t="str">
         <f t="shared" ref="J37" si="1">_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J4," IOSTANDARD LVDS_25} [get_ports ",O4,"]; #",K4)</f>
-        <v>set_property -dict {PACKAGE_PIN V4 IOSTANDARD LVDS_25} [get_ports Ch[1][0][0]]; #B13_L21_N</v>
+        <v>set_property -dict {PACKAGE_PIN V4 IOSTANDARD LVDS_25} [get_ports Ch_B_N[0]]; #B13_L21_N</v>
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B5," IOSTANDARD LVDS_25} [get_ports ",G5,"]; #",C5)</f>
-        <v>set_property -dict {PACKAGE_PIN G17 IOSTANDARD LVDS_25} [get_ports Ch[0][1][1]]; #B35_L6_P</v>
+        <v>set_property -dict {PACKAGE_PIN G17 IOSTANDARD LVDS_25} [get_ports Ch_A_P[1]]; #B35_L6_P</v>
       </c>
       <c r="J39" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J5," IOSTANDARD LVDS_25} [get_ports ",O5,"]; #",K5)</f>
-        <v>set_property -dict {PACKAGE_PIN Y4 IOSTANDARD LVDS_25} [get_ports Ch[1][1][1]]; #B13_L18_P</v>
+        <v>set_property -dict {PACKAGE_PIN Y4 IOSTANDARD LVDS_25} [get_ports Ch_B_P[1]]; #B13_L18_P</v>
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B6," IOSTANDARD LVDS_25} [get_ports ",G6,"]; #",C6)</f>
-        <v>set_property -dict {PACKAGE_PIN F17 IOSTANDARD LVDS_25} [get_ports Ch[0][1][0]]; #B35_L6_N</v>
+        <v>set_property -dict {PACKAGE_PIN F17 IOSTANDARD LVDS_25} [get_ports Ch_A_N[1]]; #B35_L6_N</v>
       </c>
       <c r="J40" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J6," IOSTANDARD LVDS_25} [get_ports ",O6,"]; #",K6)</f>
-        <v>set_property -dict {PACKAGE_PIN AA4 IOSTANDARD LVDS_25} [get_ports Ch[1][1][0]]; #B13_L18_N</v>
+        <v>set_property -dict {PACKAGE_PIN AA4 IOSTANDARD LVDS_25} [get_ports Ch_B_N[1]]; #B13_L18_N</v>
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B7," IOSTANDARD LVDS_25} [get_ports ",G7,"]; #",C7)</f>
-        <v>set_property -dict {PACKAGE_PIN E15 IOSTANDARD LVDS_25} [get_ports Ch[0][2][1]]; #B35_L3_P</v>
+        <v>set_property -dict {PACKAGE_PIN E15 IOSTANDARD LVDS_25} [get_ports Ch_A_P[2]]; #B35_L3_P</v>
       </c>
       <c r="J42" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J7," IOSTANDARD LVDS_25} [get_ports ",O7,"]; #",K7)</f>
-        <v>set_property -dict {PACKAGE_PIN U6 IOSTANDARD LVDS_25} [get_ports Ch[1][2][1]]; #B13_L22_P</v>
+        <v>set_property -dict {PACKAGE_PIN U6 IOSTANDARD LVDS_25} [get_ports Ch_B_P[2]]; #B13_L22_P</v>
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B8," IOSTANDARD LVDS_25} [get_ports ",G8,"]; #",C8)</f>
-        <v>set_property -dict {PACKAGE_PIN D15 IOSTANDARD LVDS_25} [get_ports Ch[0][2][0]]; #B35_L3_N</v>
+        <v>set_property -dict {PACKAGE_PIN D15 IOSTANDARD LVDS_25} [get_ports Ch_A_N[2]]; #B35_L3_N</v>
       </c>
       <c r="J43" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J8," IOSTANDARD LVDS_25} [get_ports ",O8,"]; #",K8)</f>
-        <v>set_property -dict {PACKAGE_PIN U5 IOSTANDARD LVDS_25} [get_ports Ch[1][2][0]]; #B13_L22_N</v>
+        <v>set_property -dict {PACKAGE_PIN U5 IOSTANDARD LVDS_25} [get_ports Ch_B_N[2]]; #B13_L22_N</v>
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B9," IOSTANDARD LVDS_25} [get_ports ",G9,"]; #",C9)</f>
-        <v>set_property -dict {PACKAGE_PIN F18 IOSTANDARD LVDS_25} [get_ports Ch[0][3][1]]; #B35_L5_P</v>
+        <v>set_property -dict {PACKAGE_PIN F18 IOSTANDARD LVDS_25} [get_ports Ch_A_P[3]]; #B35_L5_P</v>
       </c>
       <c r="J45" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J9," IOSTANDARD LVDS_25} [get_ports ",O9,"]; #",K9)</f>
-        <v>set_property -dict {PACKAGE_PIN R6 IOSTANDARD LVDS_25} [get_ports Ch[1][3][1]]; #B13_L19_P</v>
+        <v>set_property -dict {PACKAGE_PIN R6 IOSTANDARD LVDS_25} [get_ports Ch_B_P[3]]; #B13_L19_P</v>
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B10," IOSTANDARD LVDS_25} [get_ports ",G10,"]; #",C10)</f>
-        <v>set_property -dict {PACKAGE_PIN E18 IOSTANDARD LVDS_25} [get_ports Ch[0][3][0]]; #B35_L5_N</v>
+        <v>set_property -dict {PACKAGE_PIN E18 IOSTANDARD LVDS_25} [get_ports Ch_A_N[3]]; #B35_L5_N</v>
       </c>
       <c r="J46" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J10," IOSTANDARD LVDS_25} [get_ports ",O10,"]; #",K10)</f>
-        <v>set_property -dict {PACKAGE_PIN T6 IOSTANDARD LVDS_25} [get_ports Ch[1][3][0]]; #B13_L19_N</v>
+        <v>set_property -dict {PACKAGE_PIN T6 IOSTANDARD LVDS_25} [get_ports Ch_B_N[3]]; #B13_L19_N</v>
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B11," IOSTANDARD LVDS_25} [get_ports ",G11,"]; #",C11)</f>
-        <v>set_property -dict {PACKAGE_PIN G19 IOSTANDARD LVDS_25} [get_ports Ch[0][4][1]]; #B35_L20_P</v>
+        <v>set_property -dict {PACKAGE_PIN G19 IOSTANDARD LVDS_25} [get_ports Ch_A_P[4]]; #B35_L20_P</v>
       </c>
       <c r="J48" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J11," IOSTANDARD LVDS_25} [get_ports ",O11,"]; #",K11)</f>
-        <v>set_property -dict {PACKAGE_PIN W6 IOSTANDARD LVDS_25} [get_ports Ch[1][4][1]]; #B13_L24_P</v>
+        <v>set_property -dict {PACKAGE_PIN W6 IOSTANDARD LVDS_25} [get_ports Ch_B_P[4]]; #B13_L24_P</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B12," IOSTANDARD LVDS_25} [get_ports ",G12,"]; #",C12)</f>
-        <v>set_property -dict {PACKAGE_PIN F19 IOSTANDARD LVDS_25} [get_ports Ch[0][4][0]]; #B35_L20_N</v>
+        <v>set_property -dict {PACKAGE_PIN F19 IOSTANDARD LVDS_25} [get_ports Ch_A_N[4]]; #B35_L20_N</v>
       </c>
       <c r="J49" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J12," IOSTANDARD LVDS_25} [get_ports ",O12,"]; #",K12)</f>
-        <v>set_property -dict {PACKAGE_PIN W5 IOSTANDARD LVDS_25} [get_ports Ch[1][4][0]]; #B13_L24_N</v>
+        <v>set_property -dict {PACKAGE_PIN W5 IOSTANDARD LVDS_25} [get_ports Ch_B_N[4]]; #B13_L24_N</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B13," IOSTANDARD LVDS_25} [get_ports ",G13,"]; #",C13)</f>
-        <v>set_property -dict {PACKAGE_PIN F21 IOSTANDARD LVDS_25} [get_ports Ch[0][5][1]]; #B35_L23_P</v>
+        <v>set_property -dict {PACKAGE_PIN F21 IOSTANDARD LVDS_25} [get_ports Ch_A_P[5]]; #B35_L23_P</v>
       </c>
       <c r="J51" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J13," IOSTANDARD LVDS_25} [get_ports ",O13,"]; #",K13)</f>
-        <v>set_property -dict {PACKAGE_PIN V7 IOSTANDARD LVDS_25} [get_ports Ch[1][5][1]]; #B13_L23_P</v>
+        <v>set_property -dict {PACKAGE_PIN V7 IOSTANDARD LVDS_25} [get_ports Ch_B_P[5]]; #B13_L23_P</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B14," IOSTANDARD LVDS_25} [get_ports ",G14,"]; #",C14)</f>
-        <v>set_property -dict {PACKAGE_PIN F22 IOSTANDARD LVDS_25} [get_ports Ch[0][5][0]]; #B35_L23_N</v>
+        <v>set_property -dict {PACKAGE_PIN F22 IOSTANDARD LVDS_25} [get_ports Ch_A_N[5]]; #B35_L23_N</v>
       </c>
       <c r="J52" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J14," IOSTANDARD LVDS_25} [get_ports ",O14,"]; #",K14)</f>
-        <v>set_property -dict {PACKAGE_PIN W7 IOSTANDARD LVDS_25} [get_ports Ch[1][5][0]]; #B13_L23_N</v>
+        <v>set_property -dict {PACKAGE_PIN W7 IOSTANDARD LVDS_25} [get_ports Ch_B_N[5]]; #B13_L23_N</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B15," IOSTANDARD LVDS_25} [get_ports ",G15,"]; #",C15)</f>
-        <v>set_property -dict {PACKAGE_PIN G15 IOSTANDARD LVDS_25} [get_ports Ch[0][6][1]]; #B35_L4_P</v>
+        <v>set_property -dict {PACKAGE_PIN G15 IOSTANDARD LVDS_25} [get_ports Ch_A_P[6]]; #B35_L4_P</v>
       </c>
       <c r="J54" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J15," IOSTANDARD LVDS_25} [get_ports ",O15,"]; #",K15)</f>
-        <v>set_property -dict {PACKAGE_PIN V8 IOSTANDARD LVDS_25} [get_ports Ch[1][6][1]]; #B13_L2_P</v>
+        <v>set_property -dict {PACKAGE_PIN V8 IOSTANDARD LVDS_25} [get_ports Ch_B_P[6]]; #B13_L2_P</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B16," IOSTANDARD LVDS_25} [get_ports ",G16,"]; #",C16)</f>
-        <v>set_property -dict {PACKAGE_PIN G16 IOSTANDARD LVDS_25} [get_ports Ch[0][6][0]]; #B35_L4_N</v>
+        <v>set_property -dict {PACKAGE_PIN G16 IOSTANDARD LVDS_25} [get_ports Ch_A_N[6]]; #B35_L4_N</v>
       </c>
       <c r="J55" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J16," IOSTANDARD LVDS_25} [get_ports ",O16,"]; #",K16)</f>
-        <v>set_property -dict {PACKAGE_PIN W8 IOSTANDARD LVDS_25} [get_ports Ch[1][6][0]]; #B13_L2_N</v>
+        <v>set_property -dict {PACKAGE_PIN W8 IOSTANDARD LVDS_25} [get_ports Ch_B_N[6]]; #B13_L2_N</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B17," IOSTANDARD LVDS_25} [get_ports ",G17,"]; #",C17)</f>
-        <v>set_property -dict {PACKAGE_PIN C17 IOSTANDARD LVDS_25} [get_ports Ch[0][7][1]]; #B35_L11_P</v>
+        <v>set_property -dict {PACKAGE_PIN C17 IOSTANDARD LVDS_25} [get_ports Ch_A_P[7]]; #B35_L11_P</v>
       </c>
       <c r="J57" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J17," IOSTANDARD LVDS_25} [get_ports ",O17,"]; #",K17)</f>
-        <v>set_property -dict {PACKAGE_PIN Y11 IOSTANDARD LVDS_25} [get_ports Ch[1][7][1]]; #B13_L10_P</v>
+        <v>set_property -dict {PACKAGE_PIN Y11 IOSTANDARD LVDS_25} [get_ports Ch_B_P[7]]; #B13_L10_P</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B18," IOSTANDARD LVDS_25} [get_ports ",G18,"]; #",C18)</f>
-        <v>set_property -dict {PACKAGE_PIN C18 IOSTANDARD LVDS_25} [get_ports Ch[0][7][0]]; #B35_L11_N</v>
+        <v>set_property -dict {PACKAGE_PIN C18 IOSTANDARD LVDS_25} [get_ports Ch_A_N[7]]; #B35_L11_N</v>
       </c>
       <c r="J58" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J18," IOSTANDARD LVDS_25} [get_ports ",O18,"]; #",K18)</f>
-        <v>set_property -dict {PACKAGE_PIN Y10 IOSTANDARD LVDS_25} [get_ports Ch[1][7][0]]; #B13_L10_N</v>
+        <v>set_property -dict {PACKAGE_PIN Y10 IOSTANDARD LVDS_25} [get_ports Ch_B_N[7]]; #B13_L10_N</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B19," IOSTANDARD LVDS_25} [get_ports ",G19,"]; #",C19)</f>
-        <v>set_property -dict {PACKAGE_PIN E19 IOSTANDARD LVDS_25} [get_ports Ch[0][8][1]]; #B35_L21_P</v>
+        <v>set_property -dict {PACKAGE_PIN E19 IOSTANDARD LVDS_25} [get_ports Ch_A_P[8]]; #B35_L21_P</v>
       </c>
       <c r="J60" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J19," IOSTANDARD LVDS_25} [get_ports ",O19,"]; #",K19)</f>
-        <v>set_property -dict {PACKAGE_PIN W11 IOSTANDARD LVDS_25} [get_ports Ch[1][8][1]]; #B13_L3_P</v>
+        <v>set_property -dict {PACKAGE_PIN W11 IOSTANDARD LVDS_25} [get_ports Ch_B_P[8]]; #B13_L3_P</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B20," IOSTANDARD LVDS_25} [get_ports ",G20,"]; #",C20)</f>
-        <v>set_property -dict {PACKAGE_PIN E20 IOSTANDARD LVDS_25} [get_ports Ch[0][8][0]]; #B35_L21_N</v>
+        <v>set_property -dict {PACKAGE_PIN E20 IOSTANDARD LVDS_25} [get_ports Ch_A_N[8]]; #B35_L21_N</v>
       </c>
       <c r="J61" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J20," IOSTANDARD LVDS_25} [get_ports ",O20,"]; #",K20)</f>
-        <v>set_property -dict {PACKAGE_PIN W10 IOSTANDARD LVDS_25} [get_ports Ch[1][8][0]]; #B13_L3_N</v>
+        <v>set_property -dict {PACKAGE_PIN W10 IOSTANDARD LVDS_25} [get_ports Ch_B_N[8]]; #B13_L3_N</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B21," IOSTANDARD LVDS_25} [get_ports ",G21,"]; #",C21)</f>
-        <v>set_property -dict {PACKAGE_PIN B16 IOSTANDARD LVDS_25} [get_ports Ch[0][9][1]]; #B35_L8_P</v>
+        <v>set_property -dict {PACKAGE_PIN B16 IOSTANDARD LVDS_25} [get_ports Ch_A_P[9]]; #B35_L8_P</v>
       </c>
       <c r="J63" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J21," IOSTANDARD LVDS_25} [get_ports ",O21,"]; #",K21)</f>
-        <v>set_property -dict {PACKAGE_PIN V12 IOSTANDARD LVDS_25} [get_ports Ch[1][9][1]]; #B13_L4_P</v>
+        <v>set_property -dict {PACKAGE_PIN V12 IOSTANDARD LVDS_25} [get_ports Ch_B_P[9]]; #B13_L4_P</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B22," IOSTANDARD LVDS_25} [get_ports ",G22,"]; #",C22)</f>
-        <v>set_property -dict {PACKAGE_PIN B17 IOSTANDARD LVDS_25} [get_ports Ch[0][9][0]]; #B35_L8_N</v>
+        <v>set_property -dict {PACKAGE_PIN B17 IOSTANDARD LVDS_25} [get_ports Ch_A_N[9]]; #B35_L8_N</v>
       </c>
       <c r="J64" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J22," IOSTANDARD LVDS_25} [get_ports ",O22,"]; #",K22)</f>
-        <v>set_property -dict {PACKAGE_PIN W12 IOSTANDARD LVDS_25} [get_ports Ch[1][9][0]]; #B13_L4_N</v>
+        <v>set_property -dict {PACKAGE_PIN W12 IOSTANDARD LVDS_25} [get_ports Ch_B_N[9]]; #B13_L4_N</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B66" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B23," IOSTANDARD LVDS_25} [get_ports ",G23,"]; #",C23)</f>
-        <v>set_property -dict {PACKAGE_PIN D16 IOSTANDARD LVDS_25} [get_ports Ch[0][10][1]]; #B35_L2_P</v>
+        <v>set_property -dict {PACKAGE_PIN D16 IOSTANDARD LVDS_25} [get_ports Ch_A_P[10]]; #B35_L2_P</v>
       </c>
       <c r="J66" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J23," IOSTANDARD LVDS_25} [get_ports ",O23,"]; #",K23)</f>
-        <v>set_property -dict {PACKAGE_PIN Y6 IOSTANDARD LVDS_25} [get_ports Ch[1][10][1]]; #B13_L13_P</v>
+        <v>set_property -dict {PACKAGE_PIN Y6 IOSTANDARD LVDS_25} [get_ports Ch_B_P[10]]; #B13_L13_P</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B67" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B24," IOSTANDARD LVDS_25} [get_ports ",G24,"]; #",C24)</f>
-        <v>set_property -dict {PACKAGE_PIN D17 IOSTANDARD LVDS_25} [get_ports Ch[0][10][0]]; #B35_L2_N</v>
+        <v>set_property -dict {PACKAGE_PIN D17 IOSTANDARD LVDS_25} [get_ports Ch_A_N[10]]; #B35_L2_N</v>
       </c>
       <c r="I67" s="8"/>
       <c r="J67" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J24," IOSTANDARD LVDS_25} [get_ports ",O24,"]; #",K24)</f>
-        <v>set_property -dict {PACKAGE_PIN Y5 IOSTANDARD LVDS_25} [get_ports Ch[1][10][0]]; #B13_L13_N</v>
+        <v>set_property -dict {PACKAGE_PIN Y5 IOSTANDARD LVDS_25} [get_ports Ch_B_N[10]]; #B13_L13_N</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -5561,101 +5625,101 @@
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B69" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B25," IOSTANDARD LVDS_25} [get_ports ",G25,"]; #",C25)</f>
-        <v>set_property -dict {PACKAGE_PIN G20 IOSTANDARD LVDS_25} [get_ports Ch[0][11][1]]; #B35_L22_P</v>
+        <v>set_property -dict {PACKAGE_PIN G20 IOSTANDARD LVDS_25} [get_ports Ch_A_P[11]]; #B35_L22_P</v>
       </c>
       <c r="J69" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J25," IOSTANDARD LVDS_25} [get_ports ",O25,"]; #",K25)</f>
-        <v>set_property -dict {PACKAGE_PIN AA7 IOSTANDARD LVDS_25} [get_ports Ch[1][11][1]]; #B13_L14_P</v>
+        <v>set_property -dict {PACKAGE_PIN AA7 IOSTANDARD LVDS_25} [get_ports Ch_B_P[11]]; #B13_L14_P</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B70" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B26," IOSTANDARD LVDS_25} [get_ports ",G26,"]; #",C26)</f>
-        <v>set_property -dict {PACKAGE_PIN G21 IOSTANDARD LVDS_25} [get_ports Ch[0][11][0]]; #B35_L22_N</v>
+        <v>set_property -dict {PACKAGE_PIN G21 IOSTANDARD LVDS_25} [get_ports Ch_A_N[11]]; #B35_L22_N</v>
       </c>
       <c r="J70" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J26," IOSTANDARD LVDS_25} [get_ports ",O26,"]; #",K26)</f>
-        <v>set_property -dict {PACKAGE_PIN AA6 IOSTANDARD LVDS_25} [get_ports Ch[1][11][0]]; #B13_L14_N</v>
+        <v>set_property -dict {PACKAGE_PIN AA6 IOSTANDARD LVDS_25} [get_ports Ch_B_N[11]]; #B13_L14_N</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B72" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B27," IOSTANDARD LVDS_25} [get_ports ",G27,"]; #",C27)</f>
-        <v>set_property -dict {PACKAGE_PIN A21 IOSTANDARD LVDS_25} [get_ports Ch[0][12][1]]; #B35_L15_P</v>
+        <v>set_property -dict {PACKAGE_PIN A21 IOSTANDARD LVDS_25} [get_ports Ch_A_P[12]]; #B35_L15_P</v>
       </c>
       <c r="J72" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J27," IOSTANDARD LVDS_25} [get_ports ",O27,"]; #",K27)</f>
-        <v>set_property -dict {PACKAGE_PIN Y9 IOSTANDARD LVDS_25} [get_ports Ch[1][12][1]]; #B13_L12_P</v>
+        <v>set_property -dict {PACKAGE_PIN Y9 IOSTANDARD LVDS_25} [get_ports Ch_B_P[12]]; #B13_L12_P</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B73" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B28," IOSTANDARD LVDS_25} [get_ports ",G28,"]; #",C28)</f>
-        <v>set_property -dict {PACKAGE_PIN A22 IOSTANDARD LVDS_25} [get_ports Ch[0][12][0]]; #B35_L15_N</v>
+        <v>set_property -dict {PACKAGE_PIN A22 IOSTANDARD LVDS_25} [get_ports Ch_A_N[12]]; #B35_L15_N</v>
       </c>
       <c r="J73" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J28," IOSTANDARD LVDS_25} [get_ports ",O28,"]; #",K28)</f>
-        <v>set_property -dict {PACKAGE_PIN Y8 IOSTANDARD LVDS_25} [get_ports Ch[1][12][0]]; #B13_L12_N</v>
+        <v>set_property -dict {PACKAGE_PIN Y8 IOSTANDARD LVDS_25} [get_ports Ch_B_N[12]]; #B13_L12_N</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B75" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B29," IOSTANDARD LVDS_25} [get_ports ",G29,"]; #",C29)</f>
-        <v>set_property -dict {PACKAGE_PIN B21 IOSTANDARD LVDS_25} [get_ports Ch[0][13][1]]; #B35_L18_P</v>
+        <v>set_property -dict {PACKAGE_PIN B21 IOSTANDARD LVDS_25} [get_ports Ch_A_P[13]]; #B35_L18_P</v>
       </c>
       <c r="J75" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J29," IOSTANDARD LVDS_25} [get_ports ",O29,"]; #",K29)</f>
-        <v>set_property -dict {PACKAGE_PIN V10 IOSTANDARD LVDS_25} [get_ports Ch[1][13][1]]; #B13_L1_P</v>
+        <v>set_property -dict {PACKAGE_PIN V10 IOSTANDARD LVDS_25} [get_ports Ch_B_P[13]]; #B13_L1_P</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B76" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B30," IOSTANDARD LVDS_25} [get_ports ",G30,"]; #",C30)</f>
-        <v>set_property -dict {PACKAGE_PIN B22 IOSTANDARD LVDS_25} [get_ports Ch[0][13][0]]; #B35_L18_N</v>
+        <v>set_property -dict {PACKAGE_PIN B22 IOSTANDARD LVDS_25} [get_ports Ch_A_N[13]]; #B35_L18_N</v>
       </c>
       <c r="J76" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J30," IOSTANDARD LVDS_25} [get_ports ",O30,"]; #",K30)</f>
-        <v>set_property -dict {PACKAGE_PIN V9 IOSTANDARD LVDS_25} [get_ports Ch[1][13][0]]; #B13_L1_N</v>
+        <v>set_property -dict {PACKAGE_PIN V9 IOSTANDARD LVDS_25} [get_ports Ch_B_N[13]]; #B13_L1_N</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B78" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B31," IOSTANDARD LVDS_25} [get_ports ",G31,"]; #",C31)</f>
-        <v>set_property -dict {PACKAGE_PIN H22 IOSTANDARD LVDS_25} [get_ports Ch[0][14][1]]; #B35_L24_P</v>
+        <v>set_property -dict {PACKAGE_PIN H22 IOSTANDARD LVDS_25} [get_ports Ch_A_P[14]]; #B35_L24_P</v>
       </c>
       <c r="J78" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J31," IOSTANDARD LVDS_25} [get_ports ",O31,"]; #",K31)</f>
-        <v>set_property -dict {PACKAGE_PIN U10 IOSTANDARD LVDS_25} [get_ports Ch[1][14][1]]; #B13_L6_P</v>
+        <v>set_property -dict {PACKAGE_PIN U10 IOSTANDARD LVDS_25} [get_ports Ch_B_P[14]]; #B13_L6_P</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B79" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B32," IOSTANDARD LVDS_25} [get_ports ",G32,"]; #",C32)</f>
-        <v>set_property -dict {PACKAGE_PIN G22 IOSTANDARD LVDS_25} [get_ports Ch[0][14][0]]; #B35_L24_N</v>
+        <v>set_property -dict {PACKAGE_PIN G22 IOSTANDARD LVDS_25} [get_ports Ch_A_N[14]]; #B35_L24_N</v>
       </c>
       <c r="J79" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J32," IOSTANDARD LVDS_25} [get_ports ",O32,"]; #",K32)</f>
-        <v>set_property -dict {PACKAGE_PIN U9 IOSTANDARD LVDS_25} [get_ports Ch[1][14][0]]; #B13_L6_N</v>
+        <v>set_property -dict {PACKAGE_PIN U9 IOSTANDARD LVDS_25} [get_ports Ch_B_N[14]]; #B13_L6_N</v>
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B81" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B33," IOSTANDARD LVDS_25} [get_ports ",G33,"]; #",C33)</f>
-        <v>set_property -dict {PACKAGE_PIN A18 IOSTANDARD LVDS_25} [get_ports Ch[0][15][1]]; #B35_L10_P</v>
+        <v>set_property -dict {PACKAGE_PIN A18 IOSTANDARD LVDS_25} [get_ports Ch_A_P[15]]; #B35_L10_P</v>
       </c>
       <c r="J81" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J33," IOSTANDARD LVDS_25} [get_ports ",O33,"]; #",K33)</f>
-        <v>set_property -dict {PACKAGE_PIN U12 IOSTANDARD LVDS_25} [get_ports Ch[1][15][1]]; #B13_L5_P</v>
+        <v>set_property -dict {PACKAGE_PIN U12 IOSTANDARD LVDS_25} [get_ports Ch_B_P[15]]; #B13_L5_P</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B82" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",B34," IOSTANDARD LVDS_25} [get_ports ",G34,"]; #",C34)</f>
-        <v>set_property -dict {PACKAGE_PIN A19 IOSTANDARD LVDS_25} [get_ports Ch[0][15][0]]; #B35_L10_N</v>
+        <v>set_property -dict {PACKAGE_PIN A19 IOSTANDARD LVDS_25} [get_ports Ch_A_N[15]]; #B35_L10_N</v>
       </c>
       <c r="J82" t="str">
         <f>_xlfn.CONCAT("set_property -dict {PACKAGE_PIN ",J34," IOSTANDARD LVDS_25} [get_ports ",O34,"]; #",K34)</f>
-        <v>set_property -dict {PACKAGE_PIN U11 IOSTANDARD LVDS_25} [get_ports Ch[1][15][0]]; #B13_L5_N</v>
+        <v>set_property -dict {PACKAGE_PIN U11 IOSTANDARD LVDS_25} [get_ports Ch_B_N[15]]; #B13_L5_N</v>
       </c>
     </row>
   </sheetData>

</xml_diff>